<commit_message>
co loi chua fix: order room
</commit_message>
<xml_diff>
--- a/bug-on-fix/Bug_ StarView [4].xlsx
+++ b/bug-on-fix/Bug_ StarView [4].xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\git\15-7\resort\bug-on-fix\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bug!$A$10:$H$17</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -870,7 +875,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -905,7 +910,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1116,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,7 +1143,7 @@
       </c>
       <c r="C3" s="1">
         <f>COUNTIF(F11:F55, "Open")</f>
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1147,7 +1152,7 @@
       </c>
       <c r="C4" s="1">
         <f>COUNTIF(F11:F55, "Fix")</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1630,7 +1635,7 @@
         <v>64</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>10</v>
@@ -1728,7 +1733,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>10</v>
@@ -1746,7 +1751,7 @@
         <v>77</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>10</v>

</xml_diff>